<commit_message>
analysis for doc as article
</commit_message>
<xml_diff>
--- a/data/top_common_words.xlsx
+++ b/data/top_common_words.xlsx
@@ -25,61 +25,73 @@
     <t>hội</t>
   </si>
   <si>
+    <t>cao_tuổi</t>
+  </si>
+  <si>
     <t>chăm_sóc</t>
   </si>
   <si>
     <t>sức_khỏe</t>
   </si>
   <si>
+    <t>xã_hội</t>
+  </si>
+  <si>
     <t>tổ_chức</t>
   </si>
   <si>
-    <t>cao_tuổi</t>
-  </si>
-  <si>
     <t>tỉnh</t>
   </si>
   <si>
-    <t>xã_hội</t>
-  </si>
-  <si>
     <t>xây_dựng</t>
   </si>
   <si>
     <t>hoạt_động</t>
   </si>
   <si>
+    <t>việt_nam</t>
+  </si>
+  <si>
+    <t>gia_đình</t>
+  </si>
+  <si>
     <t>tham_gia</t>
   </si>
   <si>
+    <t>bệnh</t>
+  </si>
+  <si>
+    <t>đồng</t>
+  </si>
+  <si>
     <t>huyện</t>
   </si>
   <si>
-    <t>gia_đình</t>
+    <t>xã</t>
   </si>
   <si>
     <t>hội_viên</t>
   </si>
   <si>
-    <t>đồng</t>
-  </si>
-  <si>
-    <t>xã</t>
-  </si>
-  <si>
     <t>clb</t>
   </si>
   <si>
-    <t>việt_nam</t>
-  </si>
-  <si>
-    <t>bệnh</t>
+    <t>sống</t>
+  </si>
+  <si>
+    <t>giúp</t>
+  </si>
+  <si>
+    <t>cụ</t>
   </si>
   <si>
     <t>công_tác</t>
   </si>
   <si>
-    <t>sống</t>
+    <t>phát_triển</t>
+  </si>
+  <si>
+    <t>triệu</t>
   </si>
   <si>
     <t>vận_động</t>
@@ -91,121 +103,124 @@
     <t>cơ_sở</t>
   </si>
   <si>
-    <t>giúp</t>
+    <t>nâng</t>
+  </si>
+  <si>
+    <t>vai_trò</t>
   </si>
   <si>
     <t>phối_hợp</t>
   </si>
   <si>
-    <t>triệu</t>
-  </si>
-  <si>
-    <t>cụ</t>
-  </si>
-  <si>
-    <t>nâng</t>
-  </si>
-  <si>
-    <t>vai_trò</t>
-  </si>
-  <si>
-    <t>phát_triển</t>
+    <t>y_tế</t>
+  </si>
+  <si>
+    <t>kinh_tế</t>
+  </si>
+  <si>
+    <t>chương_trình</t>
   </si>
   <si>
     <t>khám</t>
   </si>
   <si>
+    <t>phát_huy</t>
+  </si>
+  <si>
+    <t>đi</t>
+  </si>
+  <si>
+    <t>chính_sách</t>
+  </si>
+  <si>
     <t>phong_trào</t>
   </si>
   <si>
-    <t>phát_huy</t>
-  </si>
-  <si>
-    <t>chương_trình</t>
-  </si>
-  <si>
     <t>bảo_vệ</t>
   </si>
   <si>
-    <t>y_tế</t>
+    <t>dân_số</t>
+  </si>
+  <si>
+    <t>lao_động</t>
   </si>
   <si>
     <t>ban</t>
   </si>
   <si>
+    <t>dân</t>
+  </si>
+  <si>
+    <t>già</t>
+  </si>
+  <si>
+    <t>văn_hóa</t>
+  </si>
+  <si>
+    <t>đảng</t>
+  </si>
+  <si>
     <t>toàn</t>
   </si>
   <si>
+    <t>cộng_đồng</t>
+  </si>
+  <si>
+    <t>phường</t>
+  </si>
+  <si>
     <t>quà</t>
   </si>
   <si>
-    <t>chính_sách</t>
-  </si>
-  <si>
-    <t>đảng</t>
-  </si>
-  <si>
-    <t>phường</t>
-  </si>
-  <si>
     <t>tích_cực</t>
   </si>
   <si>
-    <t>kinh_tế</t>
-  </si>
-  <si>
-    <t>đi</t>
-  </si>
-  <si>
-    <t>dân</t>
-  </si>
-  <si>
-    <t>cộng_đồng</t>
-  </si>
-  <si>
     <t>thành_phố</t>
   </si>
   <si>
+    <t>góp_phần</t>
+  </si>
+  <si>
+    <t>tinh_thần</t>
+  </si>
+  <si>
+    <t>triển_khai</t>
+  </si>
+  <si>
+    <t>mô_hình</t>
+  </si>
+  <si>
+    <t>hiệu_quả</t>
+  </si>
+  <si>
     <t>tặng</t>
   </si>
   <si>
+    <t>hàng</t>
+  </si>
+  <si>
     <t>chính_quyền</t>
   </si>
   <si>
-    <t>góp_phần</t>
-  </si>
-  <si>
-    <t>triển_khai</t>
-  </si>
-  <si>
-    <t>văn_hóa</t>
-  </si>
-  <si>
-    <t>mô_hình</t>
-  </si>
-  <si>
     <t>nghèo</t>
   </si>
   <si>
     <t>địa_bàn</t>
   </si>
   <si>
-    <t>tinh_thần</t>
-  </si>
-  <si>
-    <t>hiệu_quả</t>
-  </si>
-  <si>
-    <t>dân_số</t>
+    <t>cán_bộ</t>
+  </si>
+  <si>
+    <t>con_cháu</t>
   </si>
   <si>
     <t>tuyên_truyền</t>
   </si>
   <si>
-    <t>cán_bộ</t>
-  </si>
-  <si>
-    <t>lao_động</t>
+    <t>cuộc_sống</t>
+  </si>
+  <si>
+    <t>dinh_dưỡng</t>
   </si>
   <si>
     <t>ubnd</t>
@@ -214,109 +229,94 @@
     <t>quỹ</t>
   </si>
   <si>
-    <t>hàng</t>
-  </si>
-  <si>
-    <t>con_cháu</t>
+    <t>nhà_nước</t>
+  </si>
+  <si>
+    <t>ngành</t>
+  </si>
+  <si>
+    <t>đóng_góp</t>
+  </si>
+  <si>
+    <t>tiền</t>
+  </si>
+  <si>
+    <t>sản_phẩm</t>
+  </si>
+  <si>
+    <t>quy_định</t>
   </si>
   <si>
     <t>hoàn_cảnh</t>
   </si>
   <si>
+    <t>môi_trường</t>
+  </si>
+  <si>
+    <t>trung_tâm</t>
+  </si>
+  <si>
     <t>thành_viên</t>
   </si>
   <si>
-    <t>môi_trường</t>
-  </si>
-  <si>
-    <t>ngành</t>
-  </si>
-  <si>
-    <t>đóng_góp</t>
+    <t>chất_lượng</t>
+  </si>
+  <si>
+    <t>chủ_tịch</t>
+  </si>
+  <si>
+    <t>hệ_thống</t>
+  </si>
+  <si>
+    <t>trung_ương</t>
+  </si>
+  <si>
+    <t>dịch_vụ</t>
+  </si>
+  <si>
+    <t>bệnh_viện</t>
   </si>
   <si>
     <t>nhân_dân</t>
   </si>
   <si>
-    <t>tiền</t>
-  </si>
-  <si>
-    <t>nhà_nước</t>
-  </si>
-  <si>
-    <t>già</t>
-  </si>
-  <si>
-    <t>quy_định</t>
-  </si>
-  <si>
-    <t>cuộc_sống</t>
-  </si>
-  <si>
-    <t>trung_ương</t>
+    <t>thường_xuyên</t>
+  </si>
+  <si>
+    <t>điều_trị</t>
+  </si>
+  <si>
+    <t>trợ_cấp</t>
+  </si>
+  <si>
+    <t>đường</t>
+  </si>
+  <si>
+    <t>đời_sống</t>
+  </si>
+  <si>
+    <t>gương</t>
+  </si>
+  <si>
+    <t>nhiệm_vụ</t>
+  </si>
+  <si>
+    <t>thuốc</t>
+  </si>
+  <si>
+    <t>hằng</t>
   </si>
   <si>
     <t>nông_thôn</t>
   </si>
   <si>
-    <t>nhiệm_vụ</t>
-  </si>
-  <si>
-    <t>thường_xuyên</t>
-  </si>
-  <si>
-    <t>gương</t>
-  </si>
-  <si>
-    <t>chất_lượng</t>
-  </si>
-  <si>
-    <t>bệnh_viện</t>
-  </si>
-  <si>
-    <t>chủ_tịch</t>
-  </si>
-  <si>
-    <t>trung_tâm</t>
-  </si>
-  <si>
-    <t>đời_sống</t>
+    <t>vui</t>
+  </si>
+  <si>
+    <t>giai_đoạn</t>
   </si>
   <si>
     <t>hộ</t>
-  </si>
-  <si>
-    <t>chi_hội</t>
-  </si>
-  <si>
-    <t>hằng</t>
-  </si>
-  <si>
-    <t>đường</t>
-  </si>
-  <si>
-    <t>hệ_thống</t>
-  </si>
-  <si>
-    <t>an_ninh</t>
-  </si>
-  <si>
-    <t>tp</t>
-  </si>
-  <si>
-    <t>thành_lập</t>
-  </si>
-  <si>
-    <t>thị_trấn</t>
-  </si>
-  <si>
-    <t>giai_đoạn</t>
-  </si>
-  <si>
-    <t>điều_trị</t>
-  </si>
-  <si>
-    <t>vui</t>
   </si>
 </sst>
 </file>

</xml_diff>